<commit_message>
newly added iAuthor TC's
</commit_message>
<xml_diff>
--- a/download/CSVFile_details.xlsx
+++ b/download/CSVFile_details.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
   <si>
     <t>importSeqNo</t>
   </si>
@@ -96,9 +96,6 @@
   </si>
   <si>
     <t>B</t>
-  </si>
-  <si>
-    <t>A</t>
   </si>
 </sst>
 </file>
@@ -1599,7 +1596,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>552</v>
+        <v>622</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>22</v>
@@ -1667,7 +1664,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>482</v>
+        <v>639</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>25</v>
@@ -1735,7 +1732,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>495</v>
+        <v>640</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>25</v>
@@ -1750,7 +1747,7 @@
         <v>23</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H4" s="1">
         <v>8.5</v>
@@ -1803,7 +1800,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>519</v>
+        <v>641</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>25</v>
@@ -1871,7 +1868,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>538</v>
+        <v>642</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Adding new iAuthor testcases changes
</commit_message>
<xml_diff>
--- a/download/CSVFile_details.xlsx
+++ b/download/CSVFile_details.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
   <si>
     <t>importSeqNo</t>
   </si>
@@ -83,22 +83,58 @@
     <t>raschstability</t>
   </si>
   <si>
+    <t>MCQ</t>
+  </si>
+  <si>
+    <t>Nill</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
     <t>VSAQ</t>
   </si>
   <si>
-    <t>Nill</t>
-  </si>
-  <si>
-    <t>Low</t>
-  </si>
-  <si>
-    <t>MCQ</t>
+    <t>ISAWE</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Type X</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Medium</t>
   </si>
   <si>
     <t>B</t>
   </si>
   <si>
-    <t>A</t>
+    <t>T</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Type B</t>
+  </si>
+  <si>
+    <t>SAQ</t>
+  </si>
+  <si>
+    <t>SJT</t>
   </si>
 </sst>
 </file>
@@ -492,7 +528,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AMJ6"/>
+  <dimension ref="A1:AMJ15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="G12" sqref="G12"/>
@@ -1599,7 +1635,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>552</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>22</v>
@@ -1614,52 +1650,52 @@
         <v>23</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="R2" s="1">
-        <v>55.0</v>
+        <v>24</v>
+      </c>
+      <c r="H2" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="I2" s="1">
+        <v>-0.06</v>
+      </c>
+      <c r="J2" s="1">
+        <v>27.8</v>
+      </c>
+      <c r="K2" s="1">
+        <v>-0.03</v>
+      </c>
+      <c r="L2" s="1">
+        <v>25.1</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="N2" s="1">
+        <v>21.3</v>
+      </c>
+      <c r="O2" s="1">
+        <v>-0.07</v>
+      </c>
+      <c r="P2" s="1">
+        <v>17.3</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>-0.09</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>23</v>
       </c>
       <c r="T2" s="1">
-        <v>0.45</v>
+        <v>0.21</v>
       </c>
       <c r="U2" s="1">
-        <v>-0.9</v>
+        <v>2.25</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:1024">
@@ -1667,67 +1703,67 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>482</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R3" s="1">
+        <v>55.0</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T3" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="U3" s="1">
+        <v>-0.9</v>
+      </c>
+      <c r="V3" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="1">
-        <v>8.5</v>
-      </c>
-      <c r="I3" s="1">
-        <v>-0.06</v>
-      </c>
-      <c r="J3" s="1">
-        <v>27.8</v>
-      </c>
-      <c r="K3" s="1">
-        <v>-0.03</v>
-      </c>
-      <c r="L3" s="1">
-        <v>25.1</v>
-      </c>
-      <c r="M3" s="1">
-        <v>0.21</v>
-      </c>
-      <c r="N3" s="1">
-        <v>21.3</v>
-      </c>
-      <c r="O3" s="1">
-        <v>-0.07</v>
-      </c>
-      <c r="P3" s="1">
-        <v>17.3</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>-0.09</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="T3" s="1">
-        <v>0.21</v>
-      </c>
-      <c r="U3" s="1">
-        <v>2.25</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:1024">
@@ -1735,67 +1771,67 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>495</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R4" s="1">
+        <v>35.67</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T4" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="U4" s="1">
+        <v>-0.9</v>
+      </c>
+      <c r="V4" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="1">
-        <v>8.5</v>
-      </c>
-      <c r="I4" s="1">
-        <v>-0.06</v>
-      </c>
-      <c r="J4" s="1">
-        <v>27.8</v>
-      </c>
-      <c r="K4" s="1">
-        <v>-0.03</v>
-      </c>
-      <c r="L4" s="1">
-        <v>25.1</v>
-      </c>
-      <c r="M4" s="1">
-        <v>0.21</v>
-      </c>
-      <c r="N4" s="1">
-        <v>21.3</v>
-      </c>
-      <c r="O4" s="1">
-        <v>-0.07</v>
-      </c>
-      <c r="P4" s="1">
-        <v>17.3</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>-0.09</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="T4" s="1">
-        <v>0.21</v>
-      </c>
-      <c r="U4" s="1">
-        <v>2.25</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:1024">
@@ -1803,55 +1839,55 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>519</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="1">
-        <v>8.5</v>
-      </c>
-      <c r="I5" s="1">
-        <v>-0.06</v>
-      </c>
-      <c r="J5" s="1">
-        <v>27.8</v>
-      </c>
-      <c r="K5" s="1">
-        <v>-0.03</v>
-      </c>
-      <c r="L5" s="1">
-        <v>25.1</v>
-      </c>
-      <c r="M5" s="1">
-        <v>0.21</v>
-      </c>
-      <c r="N5" s="1">
-        <v>21.3</v>
-      </c>
-      <c r="O5" s="1">
-        <v>-0.07</v>
-      </c>
-      <c r="P5" s="1">
-        <v>17.3</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>-0.09</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>23</v>
+        <v>23</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R5" s="1">
+        <v>65.32</v>
       </c>
       <c r="S5" s="1" t="s">
         <v>23</v>
@@ -1860,10 +1896,10 @@
         <v>0.21</v>
       </c>
       <c r="U5" s="1">
-        <v>2.25</v>
+        <v>-0.9</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:1024">
@@ -1871,67 +1907,679 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>538</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R6" s="1">
+        <v>54.12</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T6" s="1">
+        <v>0.37</v>
+      </c>
+      <c r="U6" s="1">
+        <v>-0.9</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1024">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R7" s="1">
+        <v>38.05</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T7" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="U7" s="1">
+        <v>-0.9</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1024">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="1">
+        <v>59.9</v>
+      </c>
+      <c r="I8" s="1">
+        <v>-0.25</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T8" s="1">
+        <v>0.26</v>
+      </c>
+      <c r="U8" s="1">
+        <v>1.54</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1024">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="1">
+        <v>12.6</v>
+      </c>
+      <c r="K9" s="1">
+        <v>-0.28</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T9" s="1">
+        <v>0.28</v>
+      </c>
+      <c r="U9" s="1">
+        <v>-0.9</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1024">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" s="1">
+        <v>39.8</v>
+      </c>
+      <c r="M10" s="1">
+        <v>0.26</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T10" s="1">
+        <v>0.28</v>
+      </c>
+      <c r="U10" s="1">
+        <v>-0.9</v>
+      </c>
+      <c r="V10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="1">
+    </row>
+    <row r="11" spans="1:1024">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N11" s="1">
+        <v>12.6</v>
+      </c>
+      <c r="O11" s="1">
+        <v>-0.28</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T11" s="1">
+        <v>0.28</v>
+      </c>
+      <c r="U11" s="1">
+        <v>-0.9</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1024">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P12" s="1">
+        <v>87.4</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>0.28</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T12" s="1">
+        <v>0.28</v>
+      </c>
+      <c r="U12" s="1">
+        <v>-0.9</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1024">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>5</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="1">
         <v>8.5</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I13" s="1">
         <v>-0.06</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J13" s="1">
         <v>27.8</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K13" s="1">
         <v>-0.03</v>
       </c>
-      <c r="L6" s="1">
+      <c r="L13" s="1">
         <v>25.1</v>
       </c>
-      <c r="M6" s="1">
+      <c r="M13" s="1">
         <v>0.21</v>
       </c>
-      <c r="N6" s="1">
+      <c r="N13" s="1">
         <v>21.3</v>
       </c>
-      <c r="O6" s="1">
+      <c r="O13" s="1">
         <v>-0.07</v>
       </c>
-      <c r="P6" s="1">
+      <c r="P13" s="1">
         <v>17.3</v>
       </c>
-      <c r="Q6" s="1">
+      <c r="Q13" s="1">
         <v>-0.09</v>
       </c>
-      <c r="R6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="T6" s="1">
+      <c r="R13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T13" s="1">
         <v>0.21</v>
       </c>
-      <c r="U6" s="1">
+      <c r="U13" s="1">
         <v>2.25</v>
       </c>
-      <c r="V6" s="1" t="s">
-        <v>24</v>
+      <c r="V13" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1024">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>6</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R14" s="1">
+        <v>55.0</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T14" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="U14" s="1">
+        <v>-0.9</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1024">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R15" s="1">
+        <v>55.0</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T15" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="U15" s="1">
+        <v>-0.9</v>
+      </c>
+      <c r="V15" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>